<commit_message>
fix: update to pongal sheets
</commit_message>
<xml_diff>
--- a/sheets/ice-ta-pongal.xlsx
+++ b/sheets/ice-ta-pongal.xlsx
@@ -34,12 +34,12 @@
     <t>https://img.youtube.com/vi/FrUdUIhVlnI/mqdefault.jpg</t>
   </si>
   <si>
+    <t>FrUdUIhVlnI</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=FrUdUIhVlnI</t>
   </si>
   <si>
-    <t>FrUdUIhVlnI</t>
-  </si>
-  <si>
     <t>simple rangoli</t>
   </si>
   <si>
@@ -49,36 +49,36 @@
     <t>https://img.youtube.com/vi/pbHegLtQM60/mqdefault.jpg</t>
   </si>
   <si>
+    <t>pbHegLtQM60</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=pbHegLtQM60</t>
   </si>
   <si>
-    <t>pbHegLtQM60</t>
-  </si>
-  <si>
     <t>Beautiful peacock rangoli designs</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/8lxpdDs_XF4/mqdefault.jpg</t>
   </si>
   <si>
+    <t>8lxpdDs_XF4</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=8lxpdDs_XF4</t>
   </si>
   <si>
-    <t>8lxpdDs_XF4</t>
-  </si>
-  <si>
     <t>Pongal Kolam Design with colours</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/T-iyeRyI_3I/mqdefault.jpg</t>
   </si>
   <si>
+    <t>T-iyeRyI_3I</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=T-iyeRyI_3I</t>
   </si>
   <si>
-    <t>T-iyeRyI_3I</t>
-  </si>
-  <si>
     <t>Nagu's Handwork</t>
   </si>
   <si>
@@ -88,12 +88,12 @@
     <t>https://img.youtube.com/vi/wJInZrPJop8/mqdefault.jpg</t>
   </si>
   <si>
+    <t>wJInZrPJop8</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=wJInZrPJop8</t>
   </si>
   <si>
-    <t>wJInZrPJop8</t>
-  </si>
-  <si>
     <t>muggulu rangoli</t>
   </si>
   <si>
@@ -103,12 +103,12 @@
     <t>https://img.youtube.com/vi/Z2aMPqQ-TIs/mqdefault.jpg</t>
   </si>
   <si>
+    <t>Z2aMPqQ-TIs</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=Z2aMPqQ-TIs</t>
   </si>
   <si>
-    <t>Z2aMPqQ-TIs</t>
-  </si>
-  <si>
     <t>easy rangoli designs</t>
   </si>
   <si>
@@ -118,24 +118,24 @@
     <t>https://img.youtube.com/vi/PFvBTC9Vmjk/mqdefault.jpg</t>
   </si>
   <si>
+    <t>PFvBTC9Vmjk</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=PFvBTC9Vmjk</t>
   </si>
   <si>
-    <t>PFvBTC9Vmjk</t>
-  </si>
-  <si>
     <t>Freehand Kolam for Margazhi</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/cCYQXSLnh9U/mqdefault.jpg</t>
   </si>
   <si>
+    <t>cCYQXSLnh9U</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=cCYQXSLnh9U</t>
   </si>
   <si>
-    <t>cCYQXSLnh9U</t>
-  </si>
-  <si>
     <t>thilagalakshmi sridharan</t>
   </si>
   <si>
@@ -145,12 +145,12 @@
     <t>https://img.youtube.com/vi/wbtMRAYeDy0/mqdefault.jpg</t>
   </si>
   <si>
+    <t>wbtMRAYeDy0</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=wbtMRAYeDy0</t>
   </si>
   <si>
-    <t>wbtMRAYeDy0</t>
-  </si>
-  <si>
     <t>Vasu Rangoli</t>
   </si>
   <si>
@@ -160,12 +160,12 @@
     <t>https://img.youtube.com/vi/vU3k4L-pUqQ/mqdefault.jpg</t>
   </si>
   <si>
+    <t>vU3k4L-pUqQ</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=vU3k4L-pUqQ</t>
   </si>
   <si>
-    <t>vU3k4L-pUqQ</t>
-  </si>
-  <si>
     <t>Easy Rangoli Designs</t>
   </si>
   <si>
@@ -175,24 +175,24 @@
     <t>https://img.youtube.com/vi/SpvzpOQFDmU/mqdefault.jpg</t>
   </si>
   <si>
+    <t>SpvzpOQFDmU</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=SpvzpOQFDmU</t>
   </si>
   <si>
-    <t>SpvzpOQFDmU</t>
-  </si>
-  <si>
     <t>pongal kolam with colours</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/L_W-UjKHLPA/mqdefault.jpg</t>
   </si>
   <si>
+    <t>L_W-UjKHLPA</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=L_W-UjKHLPA</t>
   </si>
   <si>
-    <t>L_W-UjKHLPA</t>
-  </si>
-  <si>
     <t>Rangoli designs with colours</t>
   </si>
   <si>
@@ -202,24 +202,24 @@
     <t>https://img.youtube.com/vi/T3XdaHh6FoU/mqdefault.jpg</t>
   </si>
   <si>
+    <t>T3XdaHh6FoU</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=T3XdaHh6FoU</t>
   </si>
   <si>
-    <t>T3XdaHh6FoU</t>
-  </si>
-  <si>
     <t>Happy Pongal Rangoli</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/iwRz_nC1dW4/mqdefault.jpg</t>
   </si>
   <si>
+    <t>iwRz_nC1dW4</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=iwRz_nC1dW4</t>
   </si>
   <si>
-    <t>iwRz_nC1dW4</t>
-  </si>
-  <si>
     <t>latest rangoli</t>
   </si>
   <si>
@@ -229,12 +229,12 @@
     <t>https://img.youtube.com/vi/hUjO40nOVO4/mqdefault.jpg</t>
   </si>
   <si>
+    <t>hUjO40nOVO4</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=hUjO40nOVO4&amp;t=2s</t>
   </si>
   <si>
-    <t>hUjO40nOVO4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Easy Rangoli </t>
   </si>
   <si>
@@ -244,12 +244,12 @@
     <t>https://img.youtube.com/vi/fGmyouf7LC8/mqdefault.jpg</t>
   </si>
   <si>
+    <t>fGmyouf7LC8</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=fGmyouf7LC8</t>
   </si>
   <si>
-    <t>fGmyouf7LC8</t>
-  </si>
-  <si>
     <t>Teluginti Muggulu</t>
   </si>
   <si>
@@ -259,36 +259,36 @@
     <t>https://img.youtube.com/vi/i_HthOzKsis/mqdefault.jpg</t>
   </si>
   <si>
+    <t>i_HthOzKsis</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=i_HthOzKsis</t>
   </si>
   <si>
-    <t>i_HthOzKsis</t>
-  </si>
-  <si>
     <t>pongal kolam dots - 17-3-3 / even</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/r2MrJY9aohc/mqdefault.jpg</t>
   </si>
   <si>
+    <t>r2MrJY9aohc</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=r2MrJY9aohc</t>
   </si>
   <si>
-    <t>r2MrJY9aohc</t>
-  </si>
-  <si>
     <t>pongal pot with 13 Dots</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/utQBrHUvfI8/mqdefault.jpg</t>
   </si>
   <si>
+    <t>utQBrHUvfI8</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=utQBrHUvfI8</t>
   </si>
   <si>
-    <t>utQBrHUvfI8</t>
-  </si>
-  <si>
     <t>Vibhisha Kolam</t>
   </si>
   <si>
@@ -298,48 +298,48 @@
     <t>https://img.youtube.com/vi/Oxi353yi2lc/mqdefault.jpg</t>
   </si>
   <si>
+    <t>Oxi353yi2lc</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=Oxi353yi2lc</t>
   </si>
   <si>
-    <t>Oxi353yi2lc</t>
-  </si>
-  <si>
     <t>S2 Kolam</t>
   </si>
   <si>
     <t>Padi kolam - margazhi kanya kolam</t>
   </si>
   <si>
+    <t>VTHyn2UrBpY</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=VTHyn2UrBpY&amp;t=10s</t>
   </si>
   <si>
-    <t>VTHyn2UrBpY</t>
-  </si>
-  <si>
     <t>Padi Kolam</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/OaPP7G82EXA/mqdefault.jpg</t>
   </si>
   <si>
+    <t>OaPP7G82EXA</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=OaPP7G82EXA</t>
   </si>
   <si>
-    <t>OaPP7G82EXA</t>
-  </si>
-  <si>
     <t>padi kolam designs | Margazhi Friday</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/R7bpyzXz4Ys/mqdefault.jpg</t>
   </si>
   <si>
+    <t>R7bpyzXz4Ys</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=R7bpyzXz4Ys</t>
   </si>
   <si>
-    <t>R7bpyzXz4Ys</t>
-  </si>
-  <si>
     <t>Sudha Balaji - Rangoli sans dots</t>
   </si>
   <si>
@@ -349,60 +349,60 @@
     <t>https://img.youtube.com/vi/p8IhWAh9gaM/mqdefault.jpg</t>
   </si>
   <si>
+    <t>p8IhWAh9gaM</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=p8IhWAh9gaM</t>
   </si>
   <si>
-    <t>p8IhWAh9gaM</t>
-  </si>
-  <si>
     <t>lotus rangoli</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/TMaX4fFcnis/mqdefault.jpg</t>
   </si>
   <si>
+    <t>TMaX4fFcnis</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=TMaX4fFcnis</t>
   </si>
   <si>
-    <t>TMaX4fFcnis</t>
-  </si>
-  <si>
     <t>bhogi kundalu kolam | 15 to 3 Dots</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/n2o6wEePm_M/mqdefault.jpg</t>
   </si>
   <si>
+    <t>n2o6wEePm_M</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=n2o6wEePm_M&amp;list=PLKRWLFbODx6x7i2ShWMHPQ9DSoosA1-dz&amp;index=9</t>
   </si>
   <si>
-    <t>n2o6wEePm_M</t>
-  </si>
-  <si>
     <t>bhogi kundalu muggulu 11 to 3 Dots</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/sru-rG2ldK4/mqdefault.jpg</t>
   </si>
   <si>
+    <t>sru-rG2ldK4</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=sru-rG2ldK4&amp;list=PLKRWLFbODx6x7i2ShWMHPQ9DSoosA1-dz&amp;index=11</t>
   </si>
   <si>
-    <t>sru-rG2ldK4</t>
-  </si>
-  <si>
     <t>Sankranthi bhogi kolam | 17*17 straight dots</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/PUOfCjbxNhM/mqdefault.jpg</t>
   </si>
   <si>
+    <t>PUOfCjbxNhM</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=PUOfCjbxNhM</t>
   </si>
   <si>
-    <t>PUOfCjbxNhM</t>
-  </si>
-  <si>
     <t>easy rangoli for beginners</t>
   </si>
   <si>
@@ -412,34 +412,34 @@
     <t>https://img.youtube.com/vi/ciDQ0Fu3kBM/mqdefault.jpg</t>
   </si>
   <si>
+    <t>ciDQ0Fu3kBM</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=ciDQ0Fu3kBM</t>
   </si>
   <si>
-    <t>ciDQ0Fu3kBM</t>
-  </si>
-  <si>
     <t>Unique rangoli | 17x9 middle</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/GIUzQiIK_mw/mqdefault.jpg</t>
   </si>
   <si>
+    <t>GIUzQiIK_mw</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=GIUzQiIK_mw</t>
   </si>
   <si>
-    <t>GIUzQiIK_mw</t>
-  </si>
-  <si>
     <t>Draw Beautiful Peacock | 13x13 dots</t>
   </si>
   <si>
     <t>https://img.youtube.com/vi/gOea6z2vAG0/mqdefault.jpg</t>
   </si>
   <si>
+    <t>gOea6z2vAG0</t>
+  </si>
+  <si>
     <t>https://www.youtube.com/watch?v=gOea6z2vAG0</t>
-  </si>
-  <si>
-    <t>gOea6z2vAG0</t>
   </si>
 </sst>
 </file>
@@ -643,8 +643,8 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="35.29"/>
     <col customWidth="1" min="2" max="2" width="50.86"/>
-    <col customWidth="1" min="3" max="3" width="53.14"/>
-    <col customWidth="1" min="4" max="4" width="22.29"/>
+    <col customWidth="1" min="3" max="3" width="19.71"/>
+    <col customWidth="1" min="4" max="4" width="54.86"/>
     <col customWidth="1" min="5" max="5" width="31.14"/>
   </cols>
   <sheetData>
@@ -672,10 +672,10 @@
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -689,10 +689,10 @@
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -706,10 +706,10 @@
       <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -723,10 +723,10 @@
       <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -740,10 +740,10 @@
       <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E6" s="6" t="s">
@@ -757,10 +757,10 @@
       <c r="B7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E7" s="8" t="s">
@@ -774,10 +774,10 @@
       <c r="B8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E8" s="6" t="s">
@@ -791,10 +791,10 @@
       <c r="B9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -808,10 +808,10 @@
       <c r="B10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>45</v>
       </c>
       <c r="E10" s="6" t="s">
@@ -825,10 +825,10 @@
       <c r="B11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>50</v>
       </c>
       <c r="E11" s="9" t="s">
@@ -842,10 +842,10 @@
       <c r="B12" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>55</v>
       </c>
       <c r="E12" s="10" t="s">
@@ -859,10 +859,10 @@
       <c r="B13" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E13" s="9" t="s">
@@ -876,10 +876,10 @@
       <c r="B14" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="11" t="s">
         <v>64</v>
       </c>
       <c r="E14" s="10" t="s">
@@ -893,10 +893,10 @@
       <c r="B15" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E15" s="6" t="s">
@@ -910,10 +910,10 @@
       <c r="B16" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>73</v>
       </c>
       <c r="E16" s="7" t="s">
@@ -927,10 +927,10 @@
       <c r="B17" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>78</v>
       </c>
       <c r="E17" s="6" t="s">
@@ -944,10 +944,10 @@
       <c r="B18" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>83</v>
       </c>
       <c r="E18" s="6" t="s">
@@ -961,10 +961,10 @@
       <c r="B19" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>87</v>
       </c>
       <c r="E19" s="9" t="s">
@@ -978,10 +978,10 @@
       <c r="B20" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>91</v>
       </c>
       <c r="E20" s="6" t="s">
@@ -995,10 +995,10 @@
       <c r="B21" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>96</v>
       </c>
       <c r="E21" s="14" t="s">
@@ -1012,10 +1012,10 @@
       <c r="B22" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>100</v>
       </c>
       <c r="E22" s="14" t="s">
@@ -1029,10 +1029,10 @@
       <c r="B23" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>104</v>
       </c>
       <c r="E23" s="6" t="s">
@@ -1046,10 +1046,10 @@
       <c r="B24" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>108</v>
       </c>
       <c r="E24" s="15" t="s">
@@ -1063,10 +1063,10 @@
       <c r="B25" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>113</v>
       </c>
       <c r="E25" s="6" t="s">
@@ -1080,10 +1080,10 @@
       <c r="B26" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>117</v>
       </c>
       <c r="E26" s="6" t="s">
@@ -1097,10 +1097,10 @@
       <c r="B27" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>121</v>
       </c>
       <c r="E27" s="6" t="s">
@@ -1114,10 +1114,10 @@
       <c r="B28" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>125</v>
       </c>
       <c r="E28" s="16" t="s">
@@ -1131,10 +1131,10 @@
       <c r="B29" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>129</v>
       </c>
       <c r="E29" s="6" t="s">
@@ -1148,10 +1148,10 @@
       <c r="B30" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>134</v>
       </c>
       <c r="E30" s="17" t="s">
@@ -1165,10 +1165,10 @@
       <c r="B31" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>138</v>
       </c>
       <c r="E31" s="6" t="s">
@@ -1182,10 +1182,10 @@
       <c r="B32" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="18" t="s">
         <v>142</v>
       </c>
       <c r="E32" s="6" t="s">
@@ -6997,84 +6997,84 @@
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="C2"/>
+    <hyperlink r:id="rId2" ref="D2"/>
     <hyperlink r:id="rId3" ref="E2"/>
     <hyperlink r:id="rId4" ref="B3"/>
-    <hyperlink r:id="rId5" ref="C3"/>
+    <hyperlink r:id="rId5" ref="D3"/>
     <hyperlink r:id="rId6" ref="B4"/>
-    <hyperlink r:id="rId7" ref="C4"/>
+    <hyperlink r:id="rId7" ref="D4"/>
     <hyperlink r:id="rId8" ref="B5"/>
-    <hyperlink r:id="rId9" ref="C5"/>
+    <hyperlink r:id="rId9" ref="D5"/>
     <hyperlink r:id="rId10" ref="E5"/>
     <hyperlink r:id="rId11" ref="B6"/>
-    <hyperlink r:id="rId12" ref="C6"/>
+    <hyperlink r:id="rId12" ref="D6"/>
     <hyperlink r:id="rId13" ref="E6"/>
     <hyperlink r:id="rId14" ref="B7"/>
-    <hyperlink r:id="rId15" ref="C7"/>
+    <hyperlink r:id="rId15" ref="D7"/>
     <hyperlink r:id="rId16" ref="E7"/>
     <hyperlink r:id="rId17" ref="B8"/>
-    <hyperlink r:id="rId18" ref="C8"/>
+    <hyperlink r:id="rId18" ref="D8"/>
     <hyperlink r:id="rId19" ref="B9"/>
-    <hyperlink r:id="rId20" ref="C9"/>
+    <hyperlink r:id="rId20" ref="D9"/>
     <hyperlink r:id="rId21" ref="B10"/>
-    <hyperlink r:id="rId22" ref="C10"/>
+    <hyperlink r:id="rId22" ref="D10"/>
     <hyperlink r:id="rId23" ref="E10"/>
     <hyperlink r:id="rId24" ref="B11"/>
-    <hyperlink r:id="rId25" ref="C11"/>
+    <hyperlink r:id="rId25" ref="D11"/>
     <hyperlink r:id="rId26" ref="B12"/>
-    <hyperlink r:id="rId27" ref="C12"/>
+    <hyperlink r:id="rId27" ref="D12"/>
     <hyperlink r:id="rId28" ref="B13"/>
-    <hyperlink r:id="rId29" ref="C13"/>
+    <hyperlink r:id="rId29" ref="D13"/>
     <hyperlink r:id="rId30" ref="B14"/>
-    <hyperlink r:id="rId31" ref="C14"/>
+    <hyperlink r:id="rId31" ref="D14"/>
     <hyperlink r:id="rId32" ref="B15"/>
-    <hyperlink r:id="rId33" ref="C15"/>
+    <hyperlink r:id="rId33" ref="D15"/>
     <hyperlink r:id="rId34" ref="E15"/>
     <hyperlink r:id="rId35" ref="B16"/>
-    <hyperlink r:id="rId36" ref="C16"/>
+    <hyperlink r:id="rId36" ref="D16"/>
     <hyperlink r:id="rId37" ref="B17"/>
-    <hyperlink r:id="rId38" ref="C17"/>
+    <hyperlink r:id="rId38" ref="D17"/>
     <hyperlink r:id="rId39" ref="E17"/>
     <hyperlink r:id="rId40" ref="B18"/>
-    <hyperlink r:id="rId41" ref="C18"/>
+    <hyperlink r:id="rId41" ref="D18"/>
     <hyperlink r:id="rId42" ref="E18"/>
     <hyperlink r:id="rId43" ref="B19"/>
-    <hyperlink r:id="rId44" ref="C19"/>
+    <hyperlink r:id="rId44" ref="D19"/>
     <hyperlink r:id="rId45" ref="B20"/>
-    <hyperlink r:id="rId46" ref="C20"/>
+    <hyperlink r:id="rId46" ref="D20"/>
     <hyperlink r:id="rId47" ref="E20"/>
     <hyperlink r:id="rId48" ref="B21"/>
-    <hyperlink r:id="rId49" ref="C21"/>
+    <hyperlink r:id="rId49" ref="D21"/>
     <hyperlink r:id="rId50" ref="B22"/>
-    <hyperlink r:id="rId51" ref="C22"/>
+    <hyperlink r:id="rId51" ref="D22"/>
     <hyperlink r:id="rId52" ref="B23"/>
-    <hyperlink r:id="rId53" ref="C23"/>
+    <hyperlink r:id="rId53" ref="D23"/>
     <hyperlink r:id="rId54" ref="E23"/>
     <hyperlink r:id="rId55" ref="B24"/>
-    <hyperlink r:id="rId56" ref="C24"/>
+    <hyperlink r:id="rId56" ref="D24"/>
     <hyperlink r:id="rId57" ref="E24"/>
     <hyperlink r:id="rId58" ref="B25"/>
-    <hyperlink r:id="rId59" ref="C25"/>
+    <hyperlink r:id="rId59" ref="D25"/>
     <hyperlink r:id="rId60" ref="E25"/>
     <hyperlink r:id="rId61" ref="B26"/>
-    <hyperlink r:id="rId62" ref="C26"/>
+    <hyperlink r:id="rId62" ref="D26"/>
     <hyperlink r:id="rId63" ref="E26"/>
     <hyperlink r:id="rId64" ref="B27"/>
-    <hyperlink r:id="rId65" ref="C27"/>
+    <hyperlink r:id="rId65" ref="D27"/>
     <hyperlink r:id="rId66" ref="E27"/>
     <hyperlink r:id="rId67" ref="B28"/>
-    <hyperlink r:id="rId68" ref="C28"/>
+    <hyperlink r:id="rId68" ref="D28"/>
     <hyperlink r:id="rId69" ref="B29"/>
-    <hyperlink r:id="rId70" ref="C29"/>
+    <hyperlink r:id="rId70" ref="D29"/>
     <hyperlink r:id="rId71" ref="E29"/>
     <hyperlink r:id="rId72" ref="B30"/>
-    <hyperlink r:id="rId73" ref="C30"/>
+    <hyperlink r:id="rId73" ref="D30"/>
     <hyperlink r:id="rId74" ref="E30"/>
     <hyperlink r:id="rId75" ref="B31"/>
-    <hyperlink r:id="rId76" ref="C31"/>
+    <hyperlink r:id="rId76" ref="D31"/>
     <hyperlink r:id="rId77" ref="E31"/>
     <hyperlink r:id="rId78" ref="B32"/>
-    <hyperlink r:id="rId79" ref="C32"/>
+    <hyperlink r:id="rId79" ref="D32"/>
     <hyperlink r:id="rId80" ref="E32"/>
   </hyperlinks>
   <drawing r:id="rId81"/>

</xml_diff>